<commit_message>
Update SprintCompass Product Backlog.xlsx
</commit_message>
<xml_diff>
--- a/SprintCompass Product Backlog.xlsx
+++ b/SprintCompass Product Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5582dedf4cc5d1c8/Fanshawe college/5th term/ProjectMgmt_INFO3112/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{BF11AE1C-8D74-054A-8179-ADACAF06C0C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6E146C7-29C0-47B8-8A1B-693C34993343}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{BF11AE1C-8D74-054A-8179-ADACAF06C0C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8434E03F-BEC8-420E-B4C8-EE9DED901E5F}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="15840" xr2:uid="{53A66AC6-72BD-734E-ACB4-8DBDC80ADCA0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{53A66AC6-72BD-734E-ACB4-8DBDC80ADCA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>Identify which user stories are going to be included in a given Sprint</t>
   </si>
   <si>
-    <t>Capture/Maintain subtasks for each user story that is included in a Sprint Plan</t>
-  </si>
-  <si>
     <t>Copy any incomplete user stories (and only incomplete subtasks) from a completed sprint to a future sprint</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>Have an understanding what user stories will be part of a planned Sprint.</t>
   </si>
   <si>
-    <t>Have a detailed understanding of the work to be completed within the current Sprint.</t>
-  </si>
-  <si>
     <t>Minimize the amount of information that needs to be moved from one Sprint to another.</t>
   </si>
   <si>
@@ -138,6 +132,12 @@
   </si>
   <si>
     <t>&lt;-- 3 hours a week of work X Team size (3) X 2 weeks = 18 hours / 4 = 4.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At the end of a Sprint (for each team member) capture the actual number of hours worked and an estimate of time to complete each subtask </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Track time spent by each team member on any given user story and provide a metric for the work remaining. </t>
   </si>
 </sst>
 </file>
@@ -181,7 +181,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,6 +191,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -223,7 +229,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -245,6 +251,9 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -568,7 +577,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -586,23 +595,23 @@
         <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2">
         <v>65</v>
@@ -616,7 +625,7 @@
         <v>4.5</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -644,11 +653,11 @@
       <c r="B7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="5">
         <v>1</v>
@@ -686,7 +695,7 @@
       <c r="B9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -707,11 +716,11 @@
       <c r="B10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="10" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="5">
         <v>3</v>
@@ -721,7 +730,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>5</v>
       </c>
@@ -729,10 +738,10 @@
         <v>3</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E11" s="5">
         <v>5</v>
@@ -750,10 +759,10 @@
         <v>7</v>
       </c>
       <c r="C12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="E12" s="5">
         <v>3</v>
@@ -771,10 +780,10 @@
         <v>7</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="E13" s="5">
         <v>5</v>
@@ -784,7 +793,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>8</v>
       </c>
@@ -792,10 +801,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E14" s="5">
         <v>3</v>
@@ -813,10 +822,10 @@
         <v>7</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E15" s="5">
         <v>5</v>
@@ -834,10 +843,10 @@
         <v>8</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E16" s="5">
         <v>3</v>

</xml_diff>